<commit_message>
Assessment of ozone formation sensitivity and possible bias analysis (data deposit)
Here is the data depist for the article "Assessment of ozone formation sensitivity and possible bias analysis in an urban ambient environment using a direct measurement technique"
</commit_message>
<xml_diff>
--- a/Data deposit.xlsx
+++ b/Data deposit.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\01_文章写作\-----东莞敏感性文章\JGR_atmospheres\2025.4投稿\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\01_文章写作\-----东莞敏感性文章\JGR_atmospheres\---2025.10回复审稿人意见\---上传系统图片\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E23B9C82-5620-4B90-B603-4CE3DFAB5E70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0CD25E3-D962-48E2-AAB4-47613553E444}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="13120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="2790" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fig.1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="39">
   <si>
     <t>1a_RIR</t>
   </si>
@@ -136,6 +136,15 @@
   </si>
   <si>
     <t>P(O3)net_CH3COCH3</t>
+  </si>
+  <si>
+    <t>Under constant NOx=9.2 ppbv:</t>
+  </si>
+  <si>
+    <t>P(O3)net_modelled</t>
+  </si>
+  <si>
+    <t>VOCs concentrations set in the model (ppbv)</t>
   </si>
 </sst>
 </file>
@@ -459,7 +468,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
@@ -1377,22 +1386,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A963C326-B1C4-43C8-AA53-229F6282114A}">
-  <dimension ref="A1:M201"/>
+  <dimension ref="A1:N201"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="16" customWidth="1"/>
     <col min="5" max="5" width="25.36328125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="40.36328125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="35.453125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="25.36328125" style="2" customWidth="1"/>
-    <col min="9" max="13" width="25.36328125" customWidth="1"/>
+    <col min="6" max="6" width="35.453125" style="2" customWidth="1"/>
+    <col min="7" max="10" width="25.36328125" customWidth="1"/>
+    <col min="12" max="12" width="34.26953125" customWidth="1"/>
+    <col min="13" max="13" width="23.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -1406,212 +1416,197 @@
         <v>26</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>23</v>
+      <c r="G1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" t="s">
+        <v>20</v>
       </c>
       <c r="J1" t="s">
-        <v>25</v>
-      </c>
-      <c r="K1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="L1" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="M1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+        <v>38</v>
+      </c>
+      <c r="N1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="F2" s="2">
-        <v>2.0423199278301301</v>
-      </c>
-      <c r="G2" s="2">
         <v>0.24113268912541999</v>
       </c>
-      <c r="H2" s="2">
-        <v>-1.5600545495792899</v>
-      </c>
-      <c r="K2">
+      <c r="H2">
         <v>20.74811</v>
       </c>
-      <c r="L2">
+      <c r="I2">
         <v>0.14933755000000001</v>
       </c>
+      <c r="J2">
+        <v>6</v>
+      </c>
       <c r="M2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+        <v>39.537323800000003</v>
+      </c>
+      <c r="N2">
+        <v>25.168762829999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="F3" s="2">
-        <v>3.4892415183913599</v>
-      </c>
-      <c r="G3" s="2">
         <v>1.7552438304293401</v>
       </c>
-      <c r="H3" s="2">
-        <v>2.1246142467324199E-2</v>
-      </c>
-      <c r="K3">
+      <c r="H3">
         <v>23.02646</v>
       </c>
-      <c r="L3">
+      <c r="I3">
         <v>1.7835366669999999</v>
       </c>
+      <c r="J3">
+        <v>7</v>
+      </c>
       <c r="M3">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+        <v>30.453859040000001</v>
+      </c>
+      <c r="N3">
+        <v>25.991749800000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="F4" s="2">
-        <v>4.8822711720813796</v>
-      </c>
-      <c r="G4" s="2">
         <v>3.2032545109919002</v>
       </c>
-      <c r="H4" s="2">
-        <v>1.5242378499024201</v>
-      </c>
-      <c r="K4">
+      <c r="H4">
         <v>28.314050000000002</v>
       </c>
-      <c r="L4">
+      <c r="I4">
         <v>3.5794808329999999</v>
       </c>
+      <c r="J4">
+        <v>8</v>
+      </c>
       <c r="M4">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+        <v>23.72239428</v>
+      </c>
+      <c r="N4">
+        <v>24.259265320000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="F5" s="2">
-        <v>6.22208829366879</v>
-      </c>
-      <c r="G5" s="2">
         <v>4.5869615852970096</v>
       </c>
-      <c r="H5" s="2">
-        <v>2.9518348769252198</v>
-      </c>
-      <c r="K5">
+      <c r="H5">
         <v>30.099250000000001</v>
       </c>
-      <c r="L5">
+      <c r="I5">
         <v>9.4383576920000003</v>
       </c>
+      <c r="J5">
+        <v>9</v>
+      </c>
       <c r="M5">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+        <v>15.81492952</v>
+      </c>
+      <c r="N5">
+        <v>15.65097742</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="F6" s="2">
-        <v>7.5092500281430503</v>
-      </c>
-      <c r="G6" s="2">
         <v>5.9081314468144503</v>
       </c>
-      <c r="H6" s="2">
-        <v>4.3070128654858504</v>
-      </c>
-      <c r="K6">
+      <c r="H6">
         <v>29.796009999999999</v>
       </c>
-      <c r="L6">
+      <c r="I6">
         <v>20.63212077</v>
       </c>
+      <c r="J6">
+        <v>10</v>
+      </c>
       <c r="M6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+        <v>7.9074647599999999</v>
+      </c>
+      <c r="N6">
+        <v>9.2446694899999997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="F7" s="2">
-        <v>8.7442340560729406</v>
-      </c>
-      <c r="G7" s="2">
         <v>7.1685002751873101</v>
       </c>
-      <c r="H7" s="2">
-        <v>5.5927664943016797</v>
-      </c>
-      <c r="K7">
+      <c r="H7">
         <v>26.52936</v>
       </c>
-      <c r="L7">
+      <c r="I7">
         <v>24.712580769999999</v>
       </c>
-      <c r="M7">
+      <c r="J7">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="F8" s="2">
-        <v>9.9274846127486391</v>
-      </c>
-      <c r="G8" s="2">
         <v>8.3697742834193694</v>
       </c>
-      <c r="H8" s="2">
-        <v>6.8120639540900996</v>
-      </c>
-      <c r="K8">
+      <c r="H8">
         <v>20.94659</v>
       </c>
-      <c r="L8">
+      <c r="I8">
         <v>22.973238460000001</v>
       </c>
-      <c r="M8">
+      <c r="J8">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="F9" s="2">
-        <v>11.0594556977882</v>
-      </c>
-      <c r="G9" s="2">
         <v>9.5136299650625507</v>
       </c>
-      <c r="H9" s="2">
-        <v>7.9678042323368699</v>
-      </c>
-      <c r="K9">
+      <c r="H9">
         <v>17.876519999999999</v>
       </c>
-      <c r="L9">
+      <c r="I9">
         <v>20.52581769</v>
       </c>
-      <c r="M9">
+      <c r="J9">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1622,25 +1617,19 @@
         <v>0.71179999999999999</v>
       </c>
       <c r="F10" s="2">
-        <v>12.1406468555623</v>
-      </c>
-      <c r="G10" s="2">
         <v>10.6017143414043</v>
       </c>
-      <c r="H10" s="2">
-        <v>9.0627818272462495</v>
-      </c>
-      <c r="K10">
+      <c r="H10">
         <v>15.33094</v>
       </c>
-      <c r="L10">
+      <c r="I10">
         <v>15.94410231</v>
       </c>
-      <c r="M10">
+      <c r="J10">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1651,25 +1640,19 @@
         <v>0.437274</v>
       </c>
       <c r="F11" s="2">
-        <v>13.171629035172399</v>
-      </c>
-      <c r="G11" s="2">
         <v>11.635645208654999</v>
       </c>
-      <c r="H11" s="2">
-        <v>10.0996613821375</v>
-      </c>
-      <c r="K11">
+      <c r="H11">
         <v>13.95163</v>
       </c>
-      <c r="L11">
+      <c r="I11">
         <v>8.8318870080000007</v>
       </c>
-      <c r="M11">
+      <c r="J11">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1680,25 +1663,19 @@
         <v>5.7000000000000002E-2</v>
       </c>
       <c r="F12" s="2">
-        <v>14.153060121512601</v>
-      </c>
-      <c r="G12" s="2">
         <v>12.617011385135401</v>
       </c>
-      <c r="H12" s="2">
-        <v>11.0809626487582</v>
-      </c>
-      <c r="K12">
+      <c r="H12">
         <v>14.276590000000001</v>
       </c>
-      <c r="L12">
+      <c r="I12">
         <v>4.4496836149999996</v>
       </c>
-      <c r="M12">
+      <c r="J12">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1709,25 +1686,19 @@
         <v>9.3490500000000004E-2</v>
       </c>
       <c r="F13" s="2">
-        <v>15.085691259927399</v>
-      </c>
-      <c r="G13" s="2">
         <v>13.5473729584641</v>
       </c>
-      <c r="H13" s="2">
-        <v>12.009054657000901</v>
-      </c>
-      <c r="K13">
+      <c r="H13">
         <v>16.162610000000001</v>
       </c>
-      <c r="L13">
+      <c r="I13">
         <v>2.0331985380000002</v>
       </c>
-      <c r="M13">
+      <c r="J13">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1738,25 +1709,19 @@
         <v>-0.121666</v>
       </c>
       <c r="F14" s="2">
-        <v>15.970365916470399</v>
-      </c>
-      <c r="G14" s="2">
         <v>14.4282615327449</v>
       </c>
-      <c r="H14" s="2">
-        <v>12.8861571490194</v>
-      </c>
-      <c r="K14">
+      <c r="H14">
         <v>17.264749999999999</v>
       </c>
-      <c r="L14">
+      <c r="I14">
         <v>0.30271843100000001</v>
       </c>
-      <c r="M14">
+      <c r="J14">
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1767,16 +1732,10 @@
         <v>-6.9846099999999897E-2</v>
       </c>
       <c r="F15" s="2">
-        <v>16.808013822690299</v>
-      </c>
-      <c r="G15" s="2">
         <v>15.261180475754101</v>
       </c>
-      <c r="H15" s="2">
-        <v>13.7143471288179</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1787,16 +1746,10 @@
         <v>-0.18976999999999999</v>
       </c>
       <c r="F16" s="2">
-        <v>17.5996417592673</v>
-      </c>
-      <c r="G16" s="2">
         <v>16.047605166128001</v>
       </c>
-      <c r="H16" s="2">
-        <v>14.4955685729887</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1807,16 +1760,10 @@
         <v>-3.9575899999999997E-2</v>
       </c>
       <c r="F17" s="2">
-        <v>18.346322745338501</v>
-      </c>
-      <c r="G17" s="2">
         <v>16.7889832405506</v>
       </c>
-      <c r="H17" s="2">
-        <v>15.231643735762701</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1827,16 +1774,10 @@
         <v>-0.29256300000000002</v>
       </c>
       <c r="F18" s="2">
-        <v>19.049184771378499</v>
-      </c>
-      <c r="G18" s="2">
         <v>17.4867348409405</v>
       </c>
-      <c r="H18" s="2">
-        <v>15.9242849105025</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1847,16 +1788,10 @@
         <v>-7.3287500000000005E-2</v>
       </c>
       <c r="F19" s="2">
-        <v>19.709399829025301</v>
-      </c>
-      <c r="G19" s="2">
         <v>18.142252861638699</v>
       </c>
-      <c r="H19" s="2">
-        <v>16.575105894252101</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1867,2022 +1802,930 @@
         <v>9.8464499999999996E-2</v>
       </c>
       <c r="F20" s="2">
-        <v>20.328173686365499</v>
-      </c>
-      <c r="G20" s="2">
         <v>18.7569031965958</v>
       </c>
-      <c r="H20" s="2">
-        <v>17.185632706825999</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>19</v>
       </c>
       <c r="F21" s="2">
-        <v>20.9067366358206</v>
-      </c>
-      <c r="G21" s="2">
         <v>19.3320249865595</v>
       </c>
-      <c r="H21" s="2">
-        <v>17.757313337298498</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>20</v>
       </c>
       <c r="F22" s="2">
-        <v>21.446335292584902</v>
-      </c>
-      <c r="G22" s="2">
         <v>19.8689308662623</v>
       </c>
-      <c r="H22" s="2">
-        <v>18.291526439939599</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>21</v>
       </c>
       <c r="F23" s="2">
-        <v>21.948225428302202</v>
-      </c>
-      <c r="G23" s="2">
         <v>20.3689072116081</v>
       </c>
-      <c r="H23" s="2">
-        <v>18.789588994913998</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>22</v>
       </c>
       <c r="F24" s="2">
-        <v>22.413665771587802</v>
-      </c>
-      <c r="G24" s="2">
         <v>20.8332143868607</v>
       </c>
-      <c r="H24" s="2">
-        <v>19.252763002133499</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>23</v>
       </c>
       <c r="F25" s="2">
-        <v>22.843912681094601</v>
-      </c>
-      <c r="G25" s="2">
         <v>21.2630869918302</v>
       </c>
-      <c r="H25" s="2">
-        <v>19.682261302565799</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>24</v>
       </c>
       <c r="F26" s="2">
-        <v>23.2402155882938</v>
-      </c>
-      <c r="G26" s="2">
         <v>21.659734109061301</v>
       </c>
-      <c r="H26" s="2">
-        <v>20.079252629828702</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="F27" s="2">
-        <v>23.603813109054801</v>
-      </c>
-      <c r="G27" s="2">
         <v>22.024339551019899</v>
       </c>
-      <c r="H27" s="2">
-        <v>20.444865992984901</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="F28" s="2">
-        <v>23.9359297308111</v>
-      </c>
-      <c r="G28" s="2">
         <v>22.3580621072811</v>
       </c>
-      <c r="H28" s="2">
-        <v>20.780194483751199</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="F29" s="2">
-        <v>24.237772992572701</v>
-      </c>
-      <c r="G29" s="2">
         <v>22.662035791716601</v>
       </c>
-      <c r="H29" s="2">
-        <v>21.086298590860501</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="F30" s="2">
-        <v>24.510531086439801</v>
-      </c>
-      <c r="G30" s="2">
         <v>22.937370089681501</v>
       </c>
-      <c r="H30" s="2">
-        <v>21.3642090929233</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="F31" s="2">
-        <v>24.755370820482501</v>
-      </c>
-      <c r="G31" s="2">
         <v>23.1851502052026</v>
       </c>
-      <c r="H31" s="2">
-        <v>21.614929589922699</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="F32" s="2">
-        <v>24.9734358932748</v>
-      </c>
-      <c r="G32" s="2">
         <v>23.406437308165099</v>
       </c>
-      <c r="H32" s="2">
-        <v>21.839438723055299</v>
-      </c>
-    </row>
-    <row r="33" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="33" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F33" s="2">
-        <v>25.165845439699599</v>
-      </c>
-      <c r="G33" s="2">
         <v>23.6022687815002</v>
       </c>
-      <c r="H33" s="2">
-        <v>22.038692123300901</v>
-      </c>
-    </row>
-    <row r="34" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="34" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F34" s="2">
-        <v>25.3336928157388</v>
-      </c>
-      <c r="G34" s="2">
         <v>23.773658468373</v>
       </c>
-      <c r="H34" s="2">
-        <v>22.213624121007101</v>
-      </c>
-    </row>
-    <row r="35" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="35" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F35" s="2">
-        <v>25.478044596815</v>
-      </c>
-      <c r="G35" s="2">
         <v>23.921596919369001</v>
       </c>
-      <c r="H35" s="2">
-        <v>22.365149241923099</v>
-      </c>
-    </row>
-    <row r="36" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="36" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F36" s="2">
-        <v>25.599939769865401</v>
-      </c>
-      <c r="G36" s="2">
         <v>24.0470516396825</v>
       </c>
-      <c r="H36" s="2">
-        <v>22.494163509499501</v>
-      </c>
-    </row>
-    <row r="37" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="37" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F37" s="2">
-        <v>25.7003891037897</v>
-      </c>
-      <c r="G37" s="2">
         <v>24.1509673363032</v>
       </c>
-      <c r="H37" s="2">
-        <v>22.601545568816601</v>
-      </c>
-    </row>
-    <row r="38" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="38" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F38" s="2">
-        <v>25.780374686267901</v>
-      </c>
-      <c r="G38" s="2">
         <v>24.234266165204101</v>
       </c>
-      <c r="H38" s="2">
-        <v>22.688157644140201</v>
-      </c>
-    </row>
-    <row r="39" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="39" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F39" s="2">
-        <v>25.8408496173132</v>
-      </c>
-      <c r="G39" s="2">
         <v>24.297847978528701</v>
       </c>
-      <c r="H39" s="2">
-        <v>22.754846339744201</v>
-      </c>
-    </row>
-    <row r="40" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="40" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F40" s="2">
-        <v>25.882737851385698</v>
-      </c>
-      <c r="G40" s="2">
         <v>24.3425905717787</v>
       </c>
-      <c r="H40" s="2">
-        <v>22.802443292171699</v>
-      </c>
-    </row>
-    <row r="41" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="41" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F41" s="2">
-        <v>25.906934180583299</v>
-      </c>
-      <c r="G41" s="2">
         <v>24.369349931000901</v>
       </c>
-      <c r="H41" s="2">
-        <v>22.831765681418499</v>
-      </c>
-    </row>
-    <row r="42" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="42" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F42" s="2">
-        <v>25.9143043514634</v>
-      </c>
-      <c r="G42" s="2">
         <v>24.378960479974999</v>
       </c>
-      <c r="H42" s="2">
-        <v>22.843616608486698</v>
-      </c>
-    </row>
-    <row r="43" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="43" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F43" s="2">
-        <v>25.905685307583401</v>
-      </c>
-      <c r="G43" s="2">
         <v>24.372235327401199</v>
       </c>
-      <c r="H43" s="2">
-        <v>22.838785347219002</v>
-      </c>
-    </row>
-    <row r="44" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="44" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F44" s="2">
-        <v>25.881885549024599</v>
-      </c>
-      <c r="G44" s="2">
         <v>24.349966514087001</v>
       </c>
-      <c r="H44" s="2">
-        <v>22.818047479149399</v>
-      </c>
-    </row>
-    <row r="45" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="45" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F45" s="2">
-        <v>25.843685599135899</v>
-      </c>
-      <c r="G45" s="2">
         <v>24.312925260135099</v>
       </c>
-      <c r="H45" s="2">
-        <v>22.782164921134299</v>
-      </c>
-    </row>
-    <row r="46" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="46" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F46" s="2">
-        <v>25.791838567645801</v>
-      </c>
-      <c r="G46" s="2">
         <v>24.261862212130701</v>
       </c>
-      <c r="H46" s="2">
-        <v>22.731885856615602</v>
-      </c>
-    </row>
-    <row r="47" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="47" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F47" s="2">
-        <v>25.727070798274202</v>
-      </c>
-      <c r="G47" s="2">
         <v>24.197507690328798</v>
       </c>
-      <c r="H47" s="2">
-        <v>22.667944582383399</v>
-      </c>
-    </row>
-    <row r="48" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="48" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F48" s="2">
-        <v>25.650082588143501</v>
-      </c>
-      <c r="G48" s="2">
         <v>24.120571935841902</v>
       </c>
-      <c r="H48" s="2">
-        <v>22.591061283540299</v>
-      </c>
-    </row>
-    <row r="49" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="49" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F49" s="2">
-        <v>25.561548965720799</v>
-      </c>
-      <c r="G49" s="2">
         <v>24.031745357826999</v>
       </c>
-      <c r="H49" s="2">
-        <v>22.501941749933099</v>
-      </c>
-    </row>
-    <row r="50" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="50" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F50" s="2">
-        <v>25.4621205137862</v>
-      </c>
-      <c r="G50" s="2">
         <v>23.931698780673301</v>
       </c>
-      <c r="H50" s="2">
-        <v>22.401277047560399</v>
-      </c>
-    </row>
-    <row r="51" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="51" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F51" s="2">
-        <v>25.352424224025398</v>
-      </c>
-      <c r="G51" s="2">
         <v>23.8210836911896</v>
       </c>
-      <c r="H51" s="2">
-        <v>22.289743158353801</v>
-      </c>
-    </row>
-    <row r="52" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="52" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F52" s="2">
-        <v>25.233064370302099</v>
-      </c>
-      <c r="G52" s="2">
         <v>23.700532485791701</v>
       </c>
-      <c r="H52" s="2">
-        <v>22.1680006012813</v>
-      </c>
-    </row>
-    <row r="53" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="53" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F53" s="2">
-        <v>25.104623388428902</v>
-      </c>
-      <c r="G53" s="2">
         <v>23.5706587176897</v>
       </c>
-      <c r="H53" s="2">
-        <v>22.036694046950402</v>
-      </c>
-    </row>
-    <row r="54" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="54" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F54" s="2">
-        <v>24.967662751298601</v>
-      </c>
-      <c r="G54" s="2">
         <v>23.432057344075499</v>
       </c>
-      <c r="H54" s="2">
-        <v>21.896451936852301</v>
-      </c>
-    </row>
-    <row r="55" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="55" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F55" s="2">
-        <v>24.822723829473698</v>
-      </c>
-      <c r="G55" s="2">
         <v>23.2853049733102</v>
       </c>
-      <c r="H55" s="2">
-        <v>21.747886117146699</v>
-      </c>
-    </row>
-    <row r="56" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="56" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F56" s="2">
-        <v>24.6703287287182</v>
-      </c>
-      <c r="G56" s="2">
         <v>23.130960112111602</v>
       </c>
-      <c r="H56" s="2">
-        <v>21.591591495505</v>
-      </c>
-    </row>
-    <row r="57" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="57" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F57" s="2">
-        <v>24.510981097404901</v>
-      </c>
-      <c r="G57" s="2">
         <v>22.9695634127415</v>
       </c>
-      <c r="H57" s="2">
-        <v>21.428145728078199</v>
-      </c>
-    </row>
-    <row r="58" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="58" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F58" s="2">
-        <v>24.345166898187401</v>
-      </c>
-      <c r="G58" s="2">
         <v>22.801637920193201</v>
       </c>
-      <c r="H58" s="2">
-        <v>21.258108942199101</v>
-      </c>
-    </row>
-    <row r="59" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="59" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F59" s="2">
-        <v>24.173355139737801</v>
-      </c>
-      <c r="G59" s="2">
         <v>22.627689319378799</v>
       </c>
-      <c r="H59" s="2">
-        <v>21.082023499019801</v>
-      </c>
-    </row>
-    <row r="60" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="60" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F60" s="2">
-        <v>23.995998565661399</v>
-      </c>
-      <c r="G60" s="2">
         <v>22.448206182316699</v>
       </c>
-      <c r="H60" s="2">
-        <v>20.900413798972</v>
-      </c>
-    </row>
-    <row r="61" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="61" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F61" s="2">
-        <v>23.813534298888001</v>
-      </c>
-      <c r="G61" s="2">
         <v>22.263660215319</v>
       </c>
-      <c r="H61" s="2">
-        <v>20.713786131749899</v>
-      </c>
-    </row>
-    <row r="62" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="62" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F62" s="2">
-        <v>23.626384440878802</v>
-      </c>
-      <c r="G62" s="2">
         <v>22.074506506178899</v>
       </c>
-      <c r="H62" s="2">
-        <v>20.522628571479</v>
-      </c>
-    </row>
-    <row r="63" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="63" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F63" s="2">
-        <v>23.4349566258613</v>
-      </c>
-      <c r="G63" s="2">
         <v>21.881183771358199</v>
       </c>
-      <c r="H63" s="2">
-        <v>20.327410916855101</v>
-      </c>
-    </row>
-    <row r="64" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="64" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F64" s="2">
-        <v>23.2396445310278</v>
-      </c>
-      <c r="G64" s="2">
         <v>21.684114603174599</v>
       </c>
-      <c r="H64" s="2">
-        <v>20.128584675321399</v>
-      </c>
-    </row>
-    <row r="65" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="65" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F65" s="2">
-        <v>23.040828344187101</v>
-      </c>
-      <c r="G65" s="2">
         <v>21.483705716989199</v>
       </c>
-      <c r="H65" s="2">
-        <v>19.926583089791301</v>
-      </c>
-    </row>
-    <row r="66" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="66" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F66" s="2">
-        <v>22.838875190780598</v>
-      </c>
-      <c r="G66" s="2">
         <v>21.280348198393799</v>
       </c>
-      <c r="H66" s="2">
-        <v>19.721821206007</v>
-      </c>
-    </row>
-    <row r="67" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="67" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F67" s="2">
-        <v>22.6341395224572</v>
-      </c>
-      <c r="G67" s="2">
         <v>21.074417750398499</v>
       </c>
-      <c r="H67" s="2">
-        <v>19.514695978339699</v>
-      </c>
-    </row>
-    <row r="68" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="68" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F68" s="2">
-        <v>22.426963469578101</v>
-      </c>
-      <c r="G68" s="2">
         <v>20.866274940618801</v>
       </c>
-      <c r="H68" s="2">
-        <v>19.305586411659402</v>
-      </c>
-    </row>
-    <row r="69" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="69" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F69" s="2">
-        <v>22.2176771600999</v>
-      </c>
-      <c r="G69" s="2">
         <v>20.656265448463401</v>
       </c>
-      <c r="H69" s="2">
-        <v>19.094853736826899</v>
-      </c>
-    </row>
-    <row r="70" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="70" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F70" s="2">
-        <v>22.006599007289999</v>
-      </c>
-      <c r="G70" s="2">
         <v>20.4447203123215</v>
       </c>
-      <c r="H70" s="2">
-        <v>18.882841617353101</v>
-      </c>
-    </row>
-    <row r="71" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="71" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F71" s="2">
-        <v>21.794035968669</v>
-      </c>
-      <c r="G71" s="2">
         <v>20.23195617675</v>
       </c>
-      <c r="H71" s="2">
-        <v>18.669876384830999</v>
-      </c>
-    </row>
-    <row r="72" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="72" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F72" s="2">
-        <v>21.580283778478002</v>
-      </c>
-      <c r="G72" s="2">
         <v>20.018275539661101</v>
       </c>
-      <c r="H72" s="2">
-        <v>18.4562673008442</v>
-      </c>
-    </row>
-    <row r="73" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="73" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F73" s="2">
-        <v>21.365627155833099</v>
-      </c>
-      <c r="G73" s="2">
         <v>19.803966999509601</v>
       </c>
-      <c r="H73" s="2">
-        <v>18.2423068431861</v>
-      </c>
-    </row>
-    <row r="74" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="74" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F74" s="2">
-        <v>21.150339990585799</v>
-      </c>
-      <c r="G74" s="2">
         <v>19.589305502480599</v>
       </c>
-      <c r="H74" s="2">
-        <v>18.028271014375498</v>
-      </c>
-    </row>
-    <row r="75" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="75" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F75" s="2">
-        <v>20.934685508746899</v>
-      </c>
-      <c r="G75" s="2">
         <v>19.3745525896766</v>
       </c>
-      <c r="H75" s="2">
-        <v>17.814419670606298</v>
-      </c>
-    </row>
-    <row r="76" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="76" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F76" s="2">
-        <v>20.7189164191808</v>
-      </c>
-      <c r="G76" s="2">
         <v>19.159956644304899</v>
       </c>
-      <c r="H76" s="2">
-        <v>17.6009968694291</v>
-      </c>
-    </row>
-    <row r="77" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="77" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F77" s="2">
-        <v>20.503275043125299</v>
-      </c>
-      <c r="G77" s="2">
         <v>18.945753138865399</v>
       </c>
-      <c r="H77" s="2">
-        <v>17.388231234605399</v>
-      </c>
-    </row>
-    <row r="78" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="78" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F78" s="2">
-        <v>20.287993427963801</v>
-      </c>
-      <c r="G78" s="2">
         <v>18.7321648823375</v>
       </c>
-      <c r="H78" s="2">
-        <v>17.176336336711199</v>
-      </c>
-    </row>
-    <row r="79" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="79" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F79" s="2">
-        <v>20.073293446557599</v>
-      </c>
-      <c r="G79" s="2">
         <v>18.519402267368001</v>
       </c>
-      <c r="H79" s="2">
-        <v>16.965511088178399</v>
-      </c>
-    </row>
-    <row r="80" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="80" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F80" s="2">
-        <v>19.8593868833572</v>
-      </c>
-      <c r="G80" s="2">
         <v>18.307663517458099</v>
       </c>
-      <c r="H80" s="2">
-        <v>16.755940151558899</v>
-      </c>
-    </row>
-    <row r="81" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="81" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F81" s="2">
-        <v>19.646475508441199</v>
-      </c>
-      <c r="G81" s="2">
         <v>18.097134934151001</v>
       </c>
-      <c r="H81" s="2">
-        <v>16.547794359860799</v>
-      </c>
-    </row>
-    <row r="82" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="82" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F82" s="2">
-        <v>19.4347511405883</v>
-      </c>
-      <c r="G82" s="2">
         <v>17.887991144219502</v>
       </c>
-      <c r="H82" s="2">
-        <v>16.341231147850799</v>
-      </c>
-    </row>
-    <row r="83" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="83" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F83" s="2">
-        <v>19.224395700474702</v>
-      </c>
-      <c r="G83" s="2">
         <v>17.680395346853199</v>
       </c>
-      <c r="H83" s="2">
-        <v>16.136394993231601</v>
-      </c>
-    </row>
-    <row r="84" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="84" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F84" s="2">
-        <v>19.015581255098098</v>
-      </c>
-      <c r="G84" s="2">
         <v>17.474499560845601</v>
       </c>
-      <c r="H84" s="2">
-        <v>15.9334178665931</v>
-      </c>
-    </row>
-    <row r="85" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="85" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F85" s="2">
-        <v>18.808470054565401</v>
-      </c>
-      <c r="G85" s="2">
         <v>17.270444871782299</v>
       </c>
-      <c r="H85" s="2">
-        <v>15.732419688999199</v>
-      </c>
-    </row>
-    <row r="86" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="86" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F86" s="2">
-        <v>18.603214562444698</v>
-      </c>
-      <c r="G86" s="2">
         <v>17.068361679227799</v>
       </c>
-      <c r="H86" s="2">
-        <v>15.533508796010899</v>
-      </c>
-    </row>
-    <row r="87" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="87" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F87" s="2">
-        <v>18.399957480960001</v>
-      </c>
-      <c r="G87" s="2">
         <v>16.868369943912999</v>
       </c>
-      <c r="H87" s="2">
-        <v>15.336782406866</v>
-      </c>
-    </row>
-    <row r="88" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="88" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F88" s="2">
-        <v>18.198831772414401</v>
-      </c>
-      <c r="G88" s="2">
         <v>16.6705794349229</v>
       </c>
-      <c r="H88" s="2">
-        <v>15.1423270974314</v>
-      </c>
-    </row>
-    <row r="89" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="89" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F89" s="2">
-        <v>17.999960678330599</v>
-      </c>
-      <c r="G89" s="2">
         <v>16.475089976883599</v>
       </c>
-      <c r="H89" s="2">
-        <v>14.9502192754366</v>
-      </c>
-    </row>
-    <row r="90" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="90" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F90" s="2">
-        <v>17.803457737935901</v>
-      </c>
-      <c r="G90" s="2">
         <v>16.281991697150101</v>
       </c>
-      <c r="H90" s="2">
-        <v>14.760525656364299</v>
-      </c>
-    </row>
-    <row r="91" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="91" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F91" s="2">
-        <v>17.609426807733101</v>
-      </c>
-      <c r="G91" s="2">
         <v>16.0913652729935</v>
       </c>
-      <c r="H91" s="2">
-        <v>14.5733037382539</v>
-      </c>
-    </row>
-    <row r="92" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="92" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F92" s="2">
-        <v>17.417962084030702</v>
-      </c>
-      <c r="G92" s="2">
         <v>15.9032821787884</v>
       </c>
-      <c r="H92" s="2">
-        <v>14.3886022735462</v>
-      </c>
-    </row>
-    <row r="93" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="93" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F93" s="2">
-        <v>17.229148130418999</v>
-      </c>
-      <c r="G93" s="2">
         <v>15.717804933200499</v>
       </c>
-      <c r="H93" s="2">
-        <v>14.206461735982</v>
-      </c>
-    </row>
-    <row r="94" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="94" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F94" s="2">
-        <v>17.043059912272799</v>
-      </c>
-      <c r="G94" s="2">
         <v>15.534987346373899</v>
       </c>
-      <c r="H94" s="2">
-        <v>14.026914780475</v>
-      </c>
-    </row>
-    <row r="95" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="95" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F95" s="2">
-        <v>16.859762840440801</v>
-      </c>
-      <c r="G95" s="2">
         <v>15.354874767118201</v>
       </c>
-      <c r="H95" s="2">
-        <v>13.8499866937956</v>
-      </c>
-    </row>
-    <row r="96" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="96" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F96" s="2">
-        <v>16.679312826322899</v>
-      </c>
-      <c r="G96" s="2">
         <v>15.177504330096699</v>
       </c>
-      <c r="H96" s="2">
-        <v>13.675695833870501</v>
-      </c>
-    </row>
-    <row r="97" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="97" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F97" s="2">
-        <v>16.501756350535</v>
-      </c>
-      <c r="G97" s="2">
         <v>15.0029052030131</v>
       </c>
-      <c r="H97" s="2">
-        <v>13.5040540554911</v>
-      </c>
-    </row>
-    <row r="98" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="98" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F98" s="2">
-        <v>16.3271305473409</v>
-      </c>
-      <c r="G98" s="2">
         <v>14.831098833799</v>
       </c>
-      <c r="H98" s="2">
-        <v>13.335067120257101</v>
-      </c>
-    </row>
-    <row r="99" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="99" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F99" s="2">
-        <v>16.155463306927398</v>
-      </c>
-      <c r="G99" s="2">
         <v>14.662099197801799</v>
       </c>
-      <c r="H99" s="2">
-        <v>13.1687350886762</v>
-      </c>
-    </row>
-    <row r="100" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="100" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F100" s="2">
-        <v>15.9867733974866</v>
-      </c>
-      <c r="G100" s="2">
         <v>14.4959130449715</v>
       </c>
-      <c r="H100" s="2">
-        <v>13.0050526924562</v>
-      </c>
-    </row>
-    <row r="101" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="101" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F101" s="2">
-        <v>15.8210706088722</v>
-      </c>
-      <c r="G101" s="2">
         <v>14.332540147048499</v>
       </c>
-      <c r="H101" s="2">
-        <v>12.8440096852247</v>
-      </c>
-    </row>
-    <row r="102" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="102" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F102" s="2">
-        <v>15.658355919383499</v>
-      </c>
-      <c r="G102" s="2">
         <v>14.171973544750999</v>
       </c>
-      <c r="H102" s="2">
-        <v>12.6855911701184</v>
-      </c>
-    </row>
-    <row r="103" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="103" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F103" s="2">
-        <v>15.4986216869464</v>
-      </c>
-      <c r="G103" s="2">
         <v>14.0141997949623</v>
       </c>
-      <c r="H103" s="2">
-        <v>12.529777902977999</v>
-      </c>
-    </row>
-    <row r="104" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="104" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F104" s="2">
-        <v>15.3418518656629</v>
-      </c>
-      <c r="G104" s="2">
         <v>13.859199217918</v>
       </c>
-      <c r="H104" s="2">
-        <v>12.376546570173099</v>
-      </c>
-    </row>
-    <row r="105" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="105" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F105" s="2">
-        <v>15.1880222483497</v>
-      </c>
-      <c r="G105" s="2">
         <v>13.706946144394101</v>
       </c>
-      <c r="H105" s="2">
-        <v>12.2258700404384</v>
-      </c>
-    </row>
-    <row r="106" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="106" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F106" s="2">
-        <v>15.037100735342801</v>
-      </c>
-      <c r="G106" s="2">
         <v>13.557409162893601</v>
       </c>
-      <c r="H106" s="2">
-        <v>12.0777175904442</v>
-      </c>
-    </row>
-    <row r="107" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="107" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F107" s="2">
-        <v>14.8890476294506</v>
-      </c>
-      <c r="G107" s="2">
         <v>13.410551366834399</v>
       </c>
-      <c r="H107" s="2">
-        <v>11.9320551042182</v>
-      </c>
-    </row>
-    <row r="108" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="108" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F108" s="2">
-        <v>14.7438159565909</v>
-      </c>
-      <c r="G108" s="2">
         <v>13.2663306017367</v>
       </c>
-      <c r="H108" s="2">
-        <v>11.7888452468825</v>
-      </c>
-    </row>
-    <row r="109" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="109" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F109" s="2">
-        <v>14.601351811262701</v>
-      </c>
-      <c r="G109" s="2">
         <v>13.124699712410299</v>
       </c>
-      <c r="H109" s="2">
-        <v>11.6480476135579</v>
-      </c>
-    </row>
-    <row r="110" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="110" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F110" s="2">
-        <v>14.461594725689601</v>
-      </c>
-      <c r="G110" s="2">
         <v>12.9856067901418</v>
       </c>
-      <c r="H110" s="2">
-        <v>11.509618854594001</v>
-      </c>
-    </row>
-    <row r="111" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="111" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F111" s="2">
-        <v>14.3244780611246</v>
-      </c>
-      <c r="G111" s="2">
         <v>12.8489954198827</v>
       </c>
-      <c r="H111" s="2">
-        <v>11.3735127786407</v>
-      </c>
-    </row>
-    <row r="112" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="112" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F112" s="2">
-        <v>14.1899294195702</v>
-      </c>
-      <c r="G112" s="2">
         <v>12.714804927435701</v>
       </c>
-      <c r="H112" s="2">
-        <v>11.239680435301301</v>
-      </c>
-    </row>
-    <row r="113" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="113" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F113" s="2">
-        <v>14.057871073902099</v>
-      </c>
-      <c r="G113" s="2">
         <v>12.582970626643601</v>
       </c>
-      <c r="H113" s="2">
-        <v>11.108070179384899</v>
-      </c>
-    </row>
-    <row r="114" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="114" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F114" s="2">
-        <v>13.928220414223601</v>
-      </c>
-      <c r="G114" s="2">
         <v>12.453424066575099</v>
       </c>
-      <c r="H114" s="2">
-        <v>10.978627718926701</v>
-      </c>
-    </row>
-    <row r="115" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="115" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F115" s="2">
-        <v>13.800890408112201</v>
-      </c>
-      <c r="G115" s="2">
         <v>12.326093278713699</v>
       </c>
-      <c r="H115" s="2">
-        <v>10.8512961493151</v>
-      </c>
-    </row>
-    <row r="116" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="116" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F116" s="2">
-        <v>13.675790072356</v>
-      </c>
-      <c r="G116" s="2">
         <v>12.2009030241438</v>
       </c>
-      <c r="H116" s="2">
-        <v>10.726015975931601</v>
-      </c>
-    </row>
-    <row r="117" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="117" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F117" s="2">
-        <v>13.552824953699</v>
-      </c>
-      <c r="G117" s="2">
         <v>12.077775040739199</v>
       </c>
-      <c r="H117" s="2">
-        <v>10.6027251277795</v>
-      </c>
-    </row>
-    <row r="118" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="118" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F118" s="2">
-        <v>13.4318976161263</v>
-      </c>
-      <c r="G118" s="2">
         <v>11.956628290349901</v>
       </c>
-      <c r="H118" s="2">
-        <v>10.4813589645736</v>
-      </c>
-    </row>
-    <row r="119" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="119" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F119" s="2">
-        <v>13.3129081322201</v>
-      </c>
-      <c r="G119" s="2">
         <v>11.837379205989601</v>
       </c>
-      <c r="H119" s="2">
-        <v>10.3618502797591</v>
-      </c>
-    </row>
-    <row r="120" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="120" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F120" s="2">
-        <v>13.1957545761875</v>
-      </c>
-      <c r="G120" s="2">
         <v>11.7199419390233</v>
       </c>
-      <c r="H120" s="2">
-        <v>10.244129301858999</v>
-      </c>
-    </row>
-    <row r="121" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="121" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F121" s="2">
-        <v>13.080333516207499</v>
-      </c>
-      <c r="G121" s="2">
         <v>11.6042286063545</v>
       </c>
-      <c r="H121" s="2">
-        <v>10.128123696501399</v>
-      </c>
-    </row>
-    <row r="122" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="122" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F122" s="2">
-        <v>12.966540503837001</v>
-      </c>
-      <c r="G122" s="2">
         <v>11.490149537612799</v>
       </c>
-      <c r="H122" s="2">
-        <v>10.013758571388401</v>
-      </c>
-    </row>
-    <row r="123" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="123" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F123" s="2">
-        <v>12.8542705582857</v>
-      </c>
-      <c r="G123" s="2">
         <v>11.377613522341001</v>
       </c>
-      <c r="H123" s="2">
-        <v>9.9009564863962698</v>
-      </c>
-    </row>
-    <row r="124" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="124" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F124" s="2">
-        <v>12.7434186434664</v>
-      </c>
-      <c r="G124" s="2">
         <v>11.2665280571831</v>
       </c>
-      <c r="H124" s="2">
-        <v>9.7896374708995797</v>
-      </c>
-    </row>
-    <row r="125" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="125" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F125" s="2">
-        <v>12.6338801357553</v>
-      </c>
-      <c r="G125" s="2">
         <v>11.156799593071201</v>
       </c>
-      <c r="H125" s="2">
-        <v>9.6797190503871899</v>
-      </c>
-    </row>
-    <row r="126" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="126" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F126" s="2">
-        <v>12.525551280507401</v>
-      </c>
-      <c r="G126" s="2">
         <v>11.0483337824129</v>
       </c>
-      <c r="H126" s="2">
-        <v>9.5711162843184194</v>
-      </c>
-    </row>
-    <row r="127" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="127" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F127" s="2">
-        <v>12.418329635353301</v>
-      </c>
-      <c r="G127" s="2">
         <v>10.941035726279299</v>
       </c>
-      <c r="H127" s="2">
-        <v>9.4637418172053192</v>
-      </c>
-    </row>
-    <row r="128" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="128" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F128" s="2">
-        <v>12.3121144983514</v>
-      </c>
-      <c r="G128" s="2">
         <v>10.834810221591599</v>
       </c>
-      <c r="H128" s="2">
-        <v>9.3575059448315994</v>
-      </c>
-    </row>
-    <row r="129" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="129" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F129" s="2">
-        <v>12.2068073190449</v>
-      </c>
-      <c r="G129" s="2">
         <v>10.729562008308999</v>
       </c>
-      <c r="H129" s="2">
-        <v>9.2523166975730398</v>
-      </c>
-    </row>
-    <row r="130" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="130" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F130" s="2">
-        <v>12.1023120904387</v>
-      </c>
-      <c r="G130" s="2">
         <v>10.625196016616201</v>
       </c>
-      <c r="H130" s="2">
-        <v>9.1480799427935509</v>
-      </c>
-    </row>
-    <row r="131" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="131" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F131" s="2">
-        <v>11.998535719861399</v>
-      </c>
-      <c r="G131" s="2">
         <v>10.5216176141105</v>
       </c>
-      <c r="H131" s="2">
-        <v>9.0446995083596295</v>
-      </c>
-    </row>
-    <row r="132" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="132" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F132" s="2">
-        <v>11.895388376627301</v>
-      </c>
-      <c r="G132" s="2">
         <v>10.4187328529894</v>
       </c>
-      <c r="H132" s="2">
-        <v>8.9420773293514006</v>
-      </c>
-    </row>
-    <row r="133" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="133" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F133" s="2">
-        <v>11.7927838143</v>
-      </c>
-      <c r="G133" s="2">
         <v>10.316448717238</v>
       </c>
-      <c r="H133" s="2">
-        <v>8.8401136201759201</v>
-      </c>
-    </row>
-    <row r="134" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="134" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F134" s="2">
-        <v>11.6906396652843</v>
-      </c>
-      <c r="G134" s="2">
         <v>10.214673369816399</v>
       </c>
-      <c r="H134" s="2">
-        <v>8.7387070743486301</v>
-      </c>
-    </row>
-    <row r="135" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="135" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F135" s="2">
-        <v>11.588877705431299</v>
-      </c>
-      <c r="G135" s="2">
         <v>10.113316399847101</v>
       </c>
-      <c r="H135" s="2">
-        <v>8.6377550942632197</v>
-      </c>
-    </row>
-    <row r="136" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="136" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F136" s="2">
-        <v>11.487424086240299</v>
-      </c>
-      <c r="G136" s="2">
         <v>10.012289069802501</v>
       </c>
-      <c r="H136" s="2">
-        <v>8.5371540533647305</v>
-      </c>
-    </row>
-    <row r="137" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="137" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F137" s="2">
-        <v>11.386209532232799</v>
-      </c>
-      <c r="G137" s="2">
         <v>9.9115045626921301</v>
       </c>
-      <c r="H137" s="2">
-        <v>8.4367995931513207</v>
-      </c>
-    </row>
-    <row r="138" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="138" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F138" s="2">
-        <v>11.2851695010883</v>
-      </c>
-      <c r="G138" s="2">
         <v>9.8108782292500294</v>
       </c>
-      <c r="H138" s="2">
-        <v>8.3365869574112992</v>
-      </c>
-    </row>
-    <row r="139" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="139" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F139" s="2">
-        <v>11.184244304249701</v>
-      </c>
-      <c r="G139" s="2">
         <v>9.7103278351224702</v>
       </c>
-      <c r="H139" s="2">
-        <v>8.2364113659952096</v>
-      </c>
-    </row>
-    <row r="140" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="140" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F140" s="2">
-        <v>11.083379185797799</v>
-      </c>
-      <c r="G140" s="2">
         <v>9.6097738080553903</v>
       </c>
-      <c r="H140" s="2">
-        <v>8.1361684303127699</v>
-      </c>
-    </row>
-    <row r="141" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="141" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F141" s="2">
-        <v>10.9825243577609</v>
-      </c>
-      <c r="G141" s="2">
         <v>9.5091394850812403</v>
       </c>
-      <c r="H141" s="2">
-        <v>8.0357546124016892</v>
-      </c>
-    </row>
-    <row r="142" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="142" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F142" s="2">
-        <v>10.8816349902919</v>
-      </c>
-      <c r="G142" s="2">
         <v>9.4083513597071704</v>
       </c>
-      <c r="H142" s="2">
-        <v>7.9350677291226104</v>
-      </c>
-    </row>
-    <row r="143" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="143" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F143" s="2">
-        <v>10.7806711557814</v>
-      </c>
-      <c r="G143" s="2">
         <v>9.3073393291018096</v>
       </c>
-      <c r="H143" s="2">
-        <v>7.8340075024222502</v>
-      </c>
-    </row>
-    <row r="144" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="144" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F144" s="2">
-        <v>10.6795977264825</v>
-      </c>
-      <c r="G144" s="2">
         <v>9.2060369412829104</v>
       </c>
-      <c r="H144" s="2">
-        <v>7.73247615608331</v>
-      </c>
-    </row>
-    <row r="145" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="145" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F145" s="2">
-        <v>10.5783842261954</v>
-      </c>
-      <c r="G145" s="2">
         <v>9.1043816423051407</v>
       </c>
-      <c r="H145" s="2">
-        <v>7.6303790584147597</v>
-      </c>
-    </row>
-    <row r="146" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="146" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F146" s="2">
-        <v>10.477004637297499</v>
-      </c>
-      <c r="G146" s="2">
         <v>9.0023150234465206</v>
       </c>
-      <c r="H146" s="2">
-        <v>7.5276254095953696</v>
-      </c>
-    </row>
-    <row r="147" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="147" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F147" s="2">
-        <v>10.3754371656684</v>
-      </c>
-      <c r="G147" s="2">
         <v>8.8997830683968804</v>
       </c>
-      <c r="H147" s="2">
-        <v>7.42412897112533</v>
-      </c>
-    </row>
-    <row r="148" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="148" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F148" s="2">
-        <v>10.273663967127</v>
-      </c>
-      <c r="G148" s="2">
         <v>8.7967364004448196</v>
       </c>
-      <c r="H148" s="2">
-        <v>7.3198088337626599</v>
-      </c>
-    </row>
-    <row r="149" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="149" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F149" s="2">
-        <v>10.171670840336001</v>
-      </c>
-      <c r="G149" s="2">
         <v>8.6931305296652805</v>
       </c>
-      <c r="H149" s="2">
-        <v>7.2145902189947</v>
-      </c>
-    </row>
-    <row r="150" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="150" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F150" s="2">
-        <v>10.069446892348701</v>
-      </c>
-      <c r="G150" s="2">
         <v>8.5889261001063399</v>
       </c>
-      <c r="H150" s="2">
-        <v>7.1084053078641203</v>
-      </c>
-    </row>
-    <row r="151" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="151" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F151" s="2">
-        <v>9.9669841844034099</v>
-      </c>
-      <c r="G151" s="2">
         <v>8.48408913697779</v>
       </c>
-      <c r="H151" s="2">
-        <v>7.0011940895523201</v>
-      </c>
-    </row>
-    <row r="152" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="152" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F152" s="2">
-        <v>9.8642773666600405</v>
-      </c>
-      <c r="G152" s="2">
         <v>8.37859129383728</v>
       </c>
-      <c r="H152" s="2">
-        <v>6.8929052210143302</v>
-      </c>
-    </row>
-    <row r="153" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="153" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F153" s="2">
-        <v>9.7613233117265903</v>
-      </c>
-      <c r="G153" s="2">
         <v>8.27241009977873</v>
       </c>
-      <c r="H153" s="2">
-        <v>6.78349688783128</v>
-      </c>
-    </row>
-    <row r="154" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="154" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F154" s="2">
-        <v>9.6581207577061399</v>
-      </c>
-      <c r="G154" s="2">
         <v>8.1655292066193397</v>
       </c>
-      <c r="H154" s="2">
-        <v>6.6729376555322402</v>
-      </c>
-    </row>
-    <row r="155" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="155" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F155" s="2">
-        <v>9.5546699720688704</v>
-      </c>
-      <c r="G155" s="2">
         <v>8.0579386360866305</v>
       </c>
-      <c r="H155" s="2">
-        <v>6.5612073001048099</v>
-      </c>
-    </row>
-    <row r="156" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="156" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F156" s="2">
-        <v>9.4509724480529993</v>
-      </c>
-      <c r="G156" s="2">
         <v>7.9496350270067904</v>
       </c>
-      <c r="H156" s="2">
-        <v>6.4482976059605797</v>
-      </c>
-    </row>
-    <row r="157" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="157" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F157" s="2">
-        <v>9.3470306451594105</v>
-      </c>
-      <c r="G157" s="2">
         <v>7.8406218824909599</v>
       </c>
-      <c r="H157" s="2">
-        <v>6.3342131198225902</v>
-      </c>
-    </row>
-    <row r="158" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="158" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F158" s="2">
-        <v>9.2428477851148703</v>
-      </c>
-      <c r="G158" s="2">
         <v>7.7309098171236901</v>
       </c>
-      <c r="H158" s="2">
-        <v>6.2189718491325001</v>
-      </c>
-    </row>
-    <row r="159" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="159" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F159" s="2">
-        <v>9.1384277137828605</v>
-      </c>
-      <c r="G159" s="2">
         <v>7.6205168041498501</v>
       </c>
-      <c r="H159" s="2">
-        <v>6.1026058945169304</v>
-      </c>
-    </row>
-    <row r="160" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="160" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F160" s="2">
-        <v>9.0337748387621009</v>
-      </c>
-      <c r="G160" s="2">
         <v>7.5094684226619801</v>
       </c>
-      <c r="H160" s="2">
-        <v>5.9851620065618798</v>
-      </c>
-    </row>
-    <row r="161" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="161" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F161" s="2">
-        <v>8.9288941510649007</v>
-      </c>
-      <c r="G161" s="2">
         <v>7.3977981047875803</v>
       </c>
-      <c r="H161" s="2">
-        <v>5.86670205851006</v>
-      </c>
-    </row>
-    <row r="162" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="162" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F162" s="2">
-        <v>8.8237913380598201</v>
-      </c>
-      <c r="G162" s="2">
         <v>7.2855473828773896</v>
       </c>
-      <c r="H162" s="2">
-        <v>5.7473034276949901</v>
-      </c>
-    </row>
-    <row r="163" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="163" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F163" s="2">
-        <v>8.7184729934789793</v>
-      </c>
-      <c r="G163" s="2">
         <v>7.1727661366913802</v>
       </c>
-      <c r="H163" s="2">
-        <v>5.6270592799043104</v>
-      </c>
-    </row>
-    <row r="164" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="164" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F164" s="2">
-        <v>8.6129469292613301</v>
-      </c>
-      <c r="G164" s="2">
         <v>7.0595128405877698</v>
       </c>
-      <c r="H164" s="2">
-        <v>5.5060787519142904</v>
-      </c>
-    </row>
-    <row r="165" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="165" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F165" s="2">
-        <v>8.5072225926727292</v>
-      </c>
-      <c r="G165" s="2">
         <v>6.9458548107090898</v>
       </c>
-      <c r="H165" s="2">
-        <v>5.3844870287451903</v>
-      </c>
-    </row>
-    <row r="166" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="166" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F166" s="2">
-        <v>8.4013115918603596</v>
-      </c>
-      <c r="G166" s="2">
         <v>6.8318684521702604</v>
       </c>
-      <c r="H166" s="2">
-        <v>5.2624253124797997</v>
-      </c>
-    </row>
-    <row r="167" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="167" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F167" s="2">
-        <v>8.2952283325257703</v>
-      </c>
-      <c r="G167" s="2">
         <v>6.7176395062456997</v>
       </c>
-      <c r="H167" s="2">
-        <v>5.1400506799661096</v>
-      </c>
-    </row>
-    <row r="168" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="168" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F168" s="2">
-        <v>8.1889907686690506</v>
-      </c>
-      <c r="G168" s="2">
         <v>6.6032632975577297</v>
       </c>
-      <c r="H168" s="2">
-        <v>5.0175358264466903</v>
-      </c>
-    </row>
-    <row r="169" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="169" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F169" s="2">
-        <v>8.0826212716148298</v>
-      </c>
-      <c r="G169" s="2">
         <v>6.4888449812622504</v>
       </c>
-      <c r="H169" s="2">
-        <v>4.8950686909097101</v>
-      </c>
-    </row>
-    <row r="170" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="170" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F170" s="2">
-        <v>7.9761476224852403</v>
-      </c>
-      <c r="G170" s="2">
         <v>6.3744997902373397</v>
       </c>
-      <c r="H170" s="2">
-        <v>4.7728519579897597</v>
-      </c>
-    </row>
-    <row r="171" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="171" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F171" s="2">
-        <v>7.8696041363070002</v>
-      </c>
-      <c r="G171" s="2">
         <v>6.2603532822707297</v>
       </c>
-      <c r="H171" s="2">
-        <v>4.6511024282347897</v>
-      </c>
-    </row>
-    <row r="172" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="172" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F172" s="2">
-        <v>7.7630329284403796</v>
-      </c>
-      <c r="G172" s="2">
         <v>6.1465415872467997</v>
       </c>
-      <c r="H172" s="2">
-        <v>4.5300502460533503</v>
-      </c>
-    </row>
-    <row r="173" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="173" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F173" s="2">
-        <v>7.65648533837361</v>
-      </c>
-      <c r="G173" s="2">
         <v>6.0332116543339298</v>
       </c>
-      <c r="H173" s="2">
-        <v>4.4099379702942096</v>
-      </c>
-    </row>
-    <row r="174" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="174" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F174" s="2">
-        <v>7.5500235303268797</v>
-      </c>
-      <c r="G174" s="2">
         <v>5.9205214991720698</v>
       </c>
-      <c r="H174" s="2">
-        <v>4.2910194680171596</v>
-      </c>
-    </row>
-    <row r="175" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="175" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F175" s="2">
-        <v>7.4437222966635996</v>
-      </c>
-      <c r="G175" s="2">
         <v>5.8086404510604002</v>
       </c>
-      <c r="H175" s="2">
-        <v>4.1735586054568499</v>
-      </c>
-    </row>
-    <row r="176" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="176" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F176" s="2">
-        <v>7.33767109590835</v>
-      </c>
-      <c r="G176" s="2">
         <v>5.69774940014445</v>
       </c>
-      <c r="H176" s="2">
-        <v>4.0578277043805597</v>
-      </c>
-    </row>
-    <row r="177" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="177" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F177" s="2">
-        <v>7.2319763663871299</v>
-      </c>
-      <c r="G177" s="2">
         <v>5.5880410446034698</v>
       </c>
-      <c r="H177" s="2">
-        <v>3.9441057228202601</v>
-      </c>
-    </row>
-    <row r="178" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="178" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F178" s="2">
-        <v>7.1267641647397504</v>
-      </c>
-      <c r="G178" s="2">
         <v>5.4797201378380702</v>
       </c>
-      <c r="H178" s="2">
-        <v>3.8326761109367</v>
-      </c>
-    </row>
-    <row r="179" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="179" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F179" s="2">
-        <v>7.0221831896255198</v>
-      </c>
-      <c r="G179" s="2">
         <v>5.3730037356578402</v>
       </c>
-      <c r="H179" s="2">
-        <v>3.72382428169005</v>
-      </c>
-    </row>
-    <row r="180" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="180" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F180" s="2">
-        <v>6.9184082621897698</v>
-      </c>
-      <c r="G180" s="2">
         <v>5.2681214434675496</v>
       </c>
-      <c r="H180" s="2">
-        <v>3.6178346247453801</v>
-      </c>
-    </row>
-    <row r="181" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="181" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F181" s="2">
-        <v>6.8156443474246799</v>
-      </c>
-      <c r="G181" s="2">
         <v>5.1653156634563002</v>
       </c>
-      <c r="H181" s="2">
-        <v>3.5149869794875399</v>
-      </c>
-    </row>
-    <row r="182" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="182" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F182" s="2">
-        <v>6.71413121295571</v>
-      </c>
-      <c r="G182" s="2">
         <v>5.0648418417839904</v>
       </c>
-      <c r="H182" s="2">
-        <v>3.4155524706124298</v>
-      </c>
-    </row>
-    <row r="183" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="183" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F183" s="2">
-        <v>6.6141488336119298</v>
-      </c>
-      <c r="G183" s="2">
         <v>4.9669687157682798</v>
       </c>
-      <c r="H183" s="2">
-        <v>3.3197885979244401</v>
-      </c>
-    </row>
-    <row r="184" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="184" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F184" s="2">
-        <v>6.5160236580272901</v>
-      </c>
-      <c r="G184" s="2">
         <v>4.8719785610733597</v>
       </c>
-      <c r="H184" s="2">
-        <v>3.22793346411934</v>
-      </c>
-    </row>
-    <row r="185" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="185" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F185" s="2">
-        <v>6.4201358556978896</v>
-      </c>
-      <c r="G185" s="2">
         <v>4.7801674388959103</v>
       </c>
-      <c r="H185" s="2">
-        <v>3.1401990220946701</v>
-      </c>
-    </row>
-    <row r="186" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="186" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F186" s="2">
-        <v>6.3269276521696796</v>
-      </c>
-      <c r="G186" s="2">
         <v>4.6918454431539498</v>
       </c>
-      <c r="H186" s="2">
-        <v>3.0567632341387001</v>
-      </c>
-    </row>
-    <row r="187" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="187" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F187" s="2">
-        <v>6.2369128288151803</v>
-      </c>
-      <c r="G187" s="2">
         <v>4.6073369476722599</v>
       </c>
-      <c r="H187" s="2">
-        <v>2.9777610665298799</v>
-      </c>
-    </row>
-    <row r="188" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="188" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F188" s="2">
-        <v>6.1506874014966897</v>
-      </c>
-      <c r="G188" s="2">
         <v>4.52698085337253</v>
       </c>
-      <c r="H188" s="2">
-        <v>2.9032743052482899</v>
-      </c>
-    </row>
-    <row r="189" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="189" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F189" s="2">
-        <v>6.0689413801313998</v>
-      </c>
-      <c r="G189" s="2">
         <v>4.4511308354578603</v>
       </c>
-      <c r="H189" s="2">
-        <v>2.8333202907847101</v>
-      </c>
-    </row>
-    <row r="190" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="190" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F190" s="2">
-        <v>5.9924713347826604</v>
-      </c>
-      <c r="G190" s="2">
         <v>4.3801555906026497</v>
       </c>
-      <c r="H190" s="2">
-        <v>2.7678398464224401</v>
-      </c>
-    </row>
-    <row r="191" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="191" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F191" s="2">
-        <v>5.9221932293945896</v>
-      </c>
-      <c r="G191" s="2">
         <v>4.3144390841382698</v>
       </c>
-      <c r="H191" s="2">
-        <v>2.7066849388823702</v>
-      </c>
-    </row>
-    <row r="192" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="192" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F192" s="2">
-        <v>5.8591546208334497</v>
-      </c>
-      <c r="G192" s="2">
         <v>4.2543807972413603</v>
       </c>
-      <c r="H192" s="2">
-        <v>2.64960697364927</v>
-      </c>
-    </row>
-    <row r="193" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="193" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F193" s="2">
-        <v>5.8045448660521304</v>
-      </c>
-      <c r="G193" s="2">
         <v>4.2003959741213501</v>
       </c>
-      <c r="H193" s="2">
-        <v>2.5962470821911601</v>
-      </c>
-    </row>
-    <row r="194" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="194" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F194" s="2">
-        <v>5.7597014768032997</v>
-      </c>
-      <c r="G194" s="2">
         <v>4.1529158692072503</v>
       </c>
-      <c r="H194" s="2">
-        <v>2.54613026161124</v>
-      </c>
-    </row>
-    <row r="195" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="195" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F195" s="2">
-        <v>5.7261103255824102</v>
-      </c>
-      <c r="G195" s="2">
         <v>4.1123879943348696</v>
       </c>
-      <c r="H195" s="2">
-        <v>2.4986656630875701</v>
-      </c>
-    </row>
-    <row r="196" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="196" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F196" s="2">
-        <v>5.7053972241395901</v>
-      </c>
-      <c r="G196" s="2">
         <v>4.0792763659360398</v>
       </c>
-      <c r="H196" s="2">
-        <v>2.4531555077331699</v>
-      </c>
-    </row>
-    <row r="197" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="197" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F197" s="2">
-        <v>5.6993087304433496</v>
-      </c>
-      <c r="G197" s="2">
         <v>4.0540617522234701</v>
       </c>
-      <c r="H197" s="2">
-        <v>2.4088147740037602</v>
-      </c>
-    </row>
-    <row r="198" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="198" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F198" s="2">
-        <v>5.70968113338356</v>
-      </c>
-      <c r="G198" s="2">
         <v>4.0372419203801302</v>
       </c>
-      <c r="H198" s="2">
-        <v>2.3648027073770801</v>
-      </c>
-    </row>
-    <row r="199" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="199" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F199" s="2">
-        <v>5.7383985029695497</v>
-      </c>
-      <c r="G199" s="2">
         <v>4.0293318837456802</v>
       </c>
-      <c r="H199" s="2">
-        <v>2.3202652645218902</v>
-      </c>
-    </row>
-    <row r="200" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="200" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F200" s="2">
-        <v>5.7873432145280903</v>
-      </c>
-      <c r="G200" s="2">
         <v>4.0308641490042998</v>
       </c>
-      <c r="H200" s="2">
-        <v>2.2743850834802402</v>
-      </c>
-    </row>
-    <row r="201" spans="6:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="201" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F201" s="2">
-        <v>5.85834477108091</v>
-      </c>
-      <c r="G201" s="2">
         <v>4.0423889633715504</v>
-      </c>
-      <c r="H201" s="2">
-        <v>2.2264331556630599</v>
       </c>
     </row>
   </sheetData>

</xml_diff>